<commit_message>
Updated excel spreadsheet with assignemnt tab
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor_solutions.xlsx
+++ b/Exercises/Perfect_Doctor_solutions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Causal-Inference/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD3E1D9-802A-EC49-9C31-13E17CE533D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC38C3-12C6-D142-8DC5-08399E3931C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="1060" windowWidth="49280" windowHeight="27160" activeTab="2" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFECT DOCTOR" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
   <si>
     <t>Person</t>
   </si>
@@ -340,6 +341,30 @@
   </si>
   <si>
     <t>should be careful about naïve correlations</t>
+  </si>
+  <si>
+    <t>Step 1: Calculate TE</t>
+  </si>
+  <si>
+    <t>Step 2: Use perfect doctor to assign D = 1 if TE&gt;0 otherwise D=0</t>
+  </si>
+  <si>
+    <t>Step 3: Use switching equation to get Y</t>
+  </si>
+  <si>
+    <t>Step 4: Calculate SDO</t>
+  </si>
+  <si>
+    <t>Step 5: Calculate selection bias, pi, ATE, ATT, ATU</t>
+  </si>
+  <si>
+    <t>Step 6: Show the decomposition of the SDO equals the sum of ATE, selection bias and heterogenous treatment effects bias</t>
+  </si>
+  <si>
+    <t>How much of the SDO is due to "causal effect" and how much is due to "selection bias"</t>
+  </si>
+  <si>
+    <t>What is selection bias now that you have gone through this exercise? Put into words that you could tell your parent and they would understand</t>
   </si>
 </sst>
 </file>
@@ -347,8 +372,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -642,7 +667,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -683,7 +708,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -699,7 +724,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1572,7 +1597,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1949,11 +1974,230 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6435EC47-A87F-0642-AAB7-EFDED12B3EB8}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>48</v>
+      </c>
+      <c r="C2" s="6">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>27</v>
+      </c>
+      <c r="C3" s="6">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6">
+        <v>33</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6">
+        <v>38</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5">
+        <v>36</v>
+      </c>
+      <c r="C8" s="6">
+        <v>29</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6">
+        <v>23</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5">
+        <v>46</v>
+      </c>
+      <c r="C10" s="6">
+        <v>34</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5">
+        <v>33</v>
+      </c>
+      <c r="C11" s="6">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6">
+        <v>27</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <v>47</v>
+      </c>
+      <c r="C13" s="6">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F0CAF-38BA-064D-B720-EB93DBD0638C}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="275" zoomScaleNormal="275" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="275" zoomScaleNormal="275" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
perfect doctor Day1 Exercise done
Uploading completed exercise of perfect doctor from Day 1
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor_solutions.xlsx
+++ b/Exercises/Perfect_Doctor_solutions.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Causal-Inference/Exercises/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.mitra\Documents\Github\Causal-Inference\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC38C3-12C6-D142-8DC5-08399E3931C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A8D6D2-47E4-47D3-AEAE-429306DC3873}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1060" windowWidth="49280" windowHeight="27160" activeTab="2" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFECT DOCTOR" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2 (2)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="115">
   <si>
     <t>Person</t>
   </si>
@@ -365,6 +368,21 @@
   </si>
   <si>
     <t>What is selection bias now that you have gone through this exercise? Put into words that you could tell your parent and they would understand</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>DECOMP</t>
+  </si>
+  <si>
+    <t>causal effect is -ve and it is -4.25, SDO also contains selection bias of -5.5, so together it becomes -9.75, but HE bias is +14, which flips the sign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selection bias here is that potential outcome for no treatment of treated units less than control units; selection bias is basically the difference in potential outcome without treatment between treated and control </t>
+  </si>
+  <si>
+    <t>it shows if treated units did not get treatment, their average outcome is different than outcome of non treated units.</t>
   </si>
 </sst>
 </file>
@@ -1041,18 +1059,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EDE92-11F1-504D-AA85-77E1FD099BAB}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="18"/>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1098,7 +1116,7 @@
       </c>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1123,7 +1141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1166,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1191,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1195,7 +1213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1220,7 +1238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1245,7 +1263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1270,7 +1288,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1295,7 +1313,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1326,7 +1344,7 @@
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1357,7 +1375,7 @@
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1382,7 +1400,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>49</v>
       </c>
@@ -1393,7 +1411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>50</v>
       </c>
@@ -1404,7 +1422,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -1417,7 +1435,7 @@
       <c r="F16"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="36">
         <f>AVERAGE(F13,F10:F11,F5,F3) - AVERAGE(F12,F6:F9,F4,F2)</f>
         <v>1.3428571428571425</v>
@@ -1440,12 +1458,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
@@ -1468,7 +1486,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <f>AVERAGE(B3,B5,B10:B11,B13)</f>
         <v>3</v>
@@ -1494,7 +1512,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -1511,7 +1529,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1519,17 +1537,17 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1537,13 +1555,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="H26" s="35"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1555,17 +1573,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1576,7 +1594,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1600,9 +1618,9 @@
       <selection sqref="A1:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1644,7 +1662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1666,7 +1684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1688,7 +1706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1710,7 +1728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1732,7 +1750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1754,7 +1772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1776,7 +1794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1820,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1864,7 +1882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1886,7 +1904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
@@ -1894,14 +1912,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <f>AVERAGE(F3,F5,F10:F11,F13) - AVERAGE(F2,F4,F6:F9,F12)</f>
         <v>1.3428571428571425</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>19</v>
       </c>
@@ -1921,7 +1939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <f>AVERAGE(B3,B5,B10:B11,B13)</f>
         <v>3</v>
@@ -1947,23 +1965,23 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>F20+ A20-B20+(1-C20)*(D20-E20)</f>
         <v>1.3428571428571425</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1975,15 +1993,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6435EC47-A87F-0642-AAB7-EFDED12B3EB8}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2002,8 +2023,18 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1">
+        <f>AVERAGE(B3,B6:B7,B11) - AVERAGE(B2,B4:B5,B8:B10,B12:B13)</f>
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2013,9 +2044,30 @@
       <c r="C2" s="6">
         <v>25</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>-23</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>E2*C2 + (1 - E2)*B2</f>
+        <v>48</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(F3,F6:F7,F11) - AVERAGE(F2,F4:F5,F8:F10,F12:F13)</f>
+        <v>4.25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K2">
+        <f>4/12</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2025,9 +2077,26 @@
       <c r="C3" s="6">
         <v>36</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">E3*C3 + (1 - E3)*B3</f>
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(D2:D13)</f>
+        <v>-4.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2037,9 +2106,26 @@
       <c r="C4" s="6">
         <v>33</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(D3,D6:D7,D11)</f>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2049,9 +2135,26 @@
       <c r="C5" s="6">
         <v>31</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(D2,D4:D5,D8:D10,D12:D13)</f>
+        <v>-11.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2061,9 +2164,19 @@
       <c r="C6" s="6">
         <v>55</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2073,9 +2186,19 @@
       <c r="C7" s="6">
         <v>38</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2085,9 +2208,26 @@
       <c r="C8" s="6">
         <v>29</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>111</v>
+      </c>
+      <c r="K8">
+        <f>K3+K1+(1-K2)*(K4 - K5)</f>
+        <v>4.2500000000000018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2097,9 +2237,19 @@
       <c r="C9" s="6">
         <v>23</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2109,9 +2259,19 @@
       <c r="C10" s="6">
         <v>34</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2121,9 +2281,19 @@
       <c r="C11" s="6">
         <v>46</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2133,9 +2303,19 @@
       <c r="C12" s="6">
         <v>27</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2145,46 +2325,71 @@
       <c r="C13" s="6">
         <v>24</v>
       </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>-23</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2196,18 +2401,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F0CAF-38BA-064D-B720-EB93DBD0638C}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScale="275" zoomScaleNormal="275" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="18"/>
-    <col min="10" max="14" width="10.83203125" style="57"/>
+    <col min="5" max="6" width="10.875" style="18"/>
+    <col min="10" max="14" width="10.875" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2435,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>6</v>
       </c>
@@ -2255,7 +2460,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>7</v>
       </c>
@@ -2283,7 +2488,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>8</v>
       </c>
@@ -2308,7 +2513,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>9</v>
       </c>
@@ -2336,7 +2541,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>10</v>
       </c>
@@ -2364,7 +2569,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>11</v>
       </c>
@@ -2389,7 +2594,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>12</v>
       </c>
@@ -2417,7 +2622,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>13</v>
       </c>
@@ -2445,7 +2650,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>14</v>
       </c>
@@ -2470,7 +2675,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>15</v>
       </c>
@@ -2498,7 +2703,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>16</v>
       </c>
@@ -2523,7 +2728,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>17</v>
       </c>
@@ -2551,7 +2756,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
         <v>101</v>
       </c>
@@ -2559,7 +2764,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>67</v>
       </c>
@@ -2588,7 +2793,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <f>AVERAGE(E2:E13)</f>
         <v>0.41666666666666669</v>
@@ -2629,7 +2834,7 @@
       <c r="M16" s="58"/>
       <c r="N16" s="58"/>
     </row>
-    <row r="17" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>90</v>
       </c>
@@ -2644,7 +2849,7 @@
       <c r="M17" s="58"/>
       <c r="N17" s="58"/>
     </row>
-    <row r="18" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="61">
         <f>C16+H16+(1-A16)*(D16-E16)</f>
         <v>-3.0285714285714285</v>
@@ -2660,7 +2865,7 @@
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
     </row>
-    <row r="19" spans="1:14" ht="37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>68</v>
       </c>
@@ -2680,17 +2885,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2701,7 +2906,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>AVERAGE(F4:F6,F8,F12)</f>
         <v>10.4</v>
@@ -2715,7 +2920,540 @@
         <v>-3.0285714285714285</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68F2B6B-73E1-42BD-BCAA-81DA0288E530}">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="18"/>
+    <col min="10" max="14" width="11" style="57"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="46">
+        <v>10</v>
+      </c>
+      <c r="C2" s="46">
+        <v>10</v>
+      </c>
+      <c r="D2" s="46">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="47">
+        <v>1</v>
+      </c>
+      <c r="F2" s="47">
+        <f>E2*C2+(1-E2)*B2</f>
+        <v>10</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="46">
+        <v>15</v>
+      </c>
+      <c r="C3" s="46">
+        <v>15</v>
+      </c>
+      <c r="D3" s="46">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="47">
+        <v>1</v>
+      </c>
+      <c r="F3" s="47">
+        <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="48">
+        <v>10</v>
+      </c>
+      <c r="C4" s="48">
+        <v>12</v>
+      </c>
+      <c r="D4" s="48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="49">
+        <v>1</v>
+      </c>
+      <c r="F4" s="47">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="48">
+        <v>8</v>
+      </c>
+      <c r="C5" s="48">
+        <v>11</v>
+      </c>
+      <c r="D5" s="48">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5" s="49">
+        <v>1</v>
+      </c>
+      <c r="F5" s="47">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="57" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="48">
+        <v>6</v>
+      </c>
+      <c r="C6" s="48">
+        <v>9</v>
+      </c>
+      <c r="D6" s="48">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E6" s="49">
+        <v>1</v>
+      </c>
+      <c r="F6" s="47">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="46">
+        <v>15</v>
+      </c>
+      <c r="C7" s="46">
+        <v>11</v>
+      </c>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E7" s="47">
+        <v>1</v>
+      </c>
+      <c r="F7" s="47">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="48">
+        <v>5</v>
+      </c>
+      <c r="C8" s="48">
+        <v>7</v>
+      </c>
+      <c r="D8" s="48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="49">
+        <v>1</v>
+      </c>
+      <c r="F8" s="47">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
+      </c>
+      <c r="J8" s="57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="46">
+        <v>13</v>
+      </c>
+      <c r="C9" s="46">
+        <v>11</v>
+      </c>
+      <c r="D9" s="46">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E9" s="47">
+        <v>1</v>
+      </c>
+      <c r="F9" s="47">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="46">
+        <v>15</v>
+      </c>
+      <c r="C10" s="46">
+        <v>6</v>
+      </c>
+      <c r="D10" s="46">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E10" s="47">
+        <v>1</v>
+      </c>
+      <c r="F10" s="47">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="46">
+        <v>11</v>
+      </c>
+      <c r="C11" s="46">
+        <v>9</v>
+      </c>
+      <c r="D11" s="46">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E11" s="47">
+        <v>1</v>
+      </c>
+      <c r="F11" s="47">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" s="57" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="48">
+        <v>10</v>
+      </c>
+      <c r="C12" s="48">
+        <v>13</v>
+      </c>
+      <c r="D12" s="48">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="49">
+        <v>0</v>
+      </c>
+      <c r="F12" s="47">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J12" s="57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="46">
+        <v>15</v>
+      </c>
+      <c r="C13" s="46">
+        <v>15</v>
+      </c>
+      <c r="D13" s="46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="47">
+        <v>0</v>
+      </c>
+      <c r="F13" s="47">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" s="57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B16" s="61">
+        <f>AVERAGE(F2:F11) - AVERAGE(F12,F13)</f>
+        <v>-2.4000000000000004</v>
+      </c>
+      <c r="C16" s="52">
+        <f>AVERAGE(D2:D13)</f>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="D16" s="54">
+        <f>AVERAGE(C2:C11)-AVERAGE(B2:B11)</f>
+        <v>-0.70000000000000107</v>
+      </c>
+      <c r="E16" s="56">
+        <f>AVERAGE(C12,C13)-AVERAGE(B12,B13)</f>
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="30">
+        <f>AVERAGE(B2:B7,B8:B10,B11)</f>
+        <v>10.8</v>
+      </c>
+      <c r="G16" s="29">
+        <f>AVERAGE(B12:B13)</f>
+        <v>12.5</v>
+      </c>
+      <c r="H16" s="29">
+        <f>F16-G16</f>
+        <v>-1.6999999999999993</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="58"/>
+    </row>
+    <row r="17" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="30"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+    </row>
+    <row r="18" spans="1:14" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="61">
+        <f>C16+H16+(1-A16)*(D16-E16)</f>
+        <v>-2.3999999999999995</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="30"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="58"/>
+    </row>
+    <row r="19" spans="1:14" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19">
+        <f>AVERAGE(C2:C13) - AVERAGE(B2:B13)</f>
+        <v>-0.33333333333333393</v>
+      </c>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>AVERAGE(F4:F6,F8,F12)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B23">
+        <f>AVERAGE(F2:F3,F7,F9:F11,F13)</f>
+        <v>11</v>
+      </c>
+      <c r="C23" s="50">
+        <f>A23-B23</f>
+        <v>-1.1999999999999993</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Changes to code and slides
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor_solutions.xlsx
+++ b/Exercises/Perfect_Doctor_solutions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Causal-Inference/Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AC38C3-12C6-D142-8DC5-08399E3931C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBF4EAE-A220-6B43-B0DF-7A8ECBF82710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1060" windowWidth="49280" windowHeight="27160" activeTab="2" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
+    <workbookView xWindow="920" yWindow="1020" windowWidth="49280" windowHeight="27160" activeTab="2" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="PERFECT DOCTOR" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="another perfect doctor example" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
   <si>
     <t>Person</t>
   </si>
@@ -365,6 +365,39 @@
   </si>
   <si>
     <t>What is selection bias now that you have gone through this exercise? Put into words that you could tell your parent and they would understand</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>SDO = ATE + E[Y0|D=1] - E[Y0|D=0] + (1-pi)(ATT-ATU)</t>
+  </si>
+  <si>
+    <t>The direct calculation of the SDO can be decomposed into three parts and when we do that</t>
+  </si>
+  <si>
+    <t>decomposition and sum those three parts we get the same answer.  And that's because</t>
+  </si>
+  <si>
+    <t>this decomposision is an identity. Not a theorem -- it must be true, and if you're not getting</t>
+  </si>
+  <si>
+    <t>that there is a mistake somewhere.</t>
+  </si>
+  <si>
+    <t>Without physical randomization, selection bias will not equal zero (usually in observational data)</t>
+  </si>
+  <si>
+    <t>and ATT will not equal ATU. And therefore SDO won't identify the ATE. SO if we are going to estimate</t>
+  </si>
+  <si>
+    <t>a causal parameter, and we can't use physical randomization, we are going to have to place</t>
+  </si>
+  <si>
+    <t>restrictions (usually) on these Y0 and Y1 potential outcomes.  And we do that in RDD, DiD, and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">synthetic control.  IV and matching and RCTs, though, use physical randomization. </t>
   </si>
 </sst>
 </file>
@@ -421,7 +454,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,8 +539,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -612,11 +651,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -725,6 +790,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1975,15 +2044,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6435EC47-A87F-0642-AAB7-EFDED12B3EB8}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2002,8 +2074,29 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2013,9 +2106,47 @@
       <c r="C2" s="6">
         <v>25</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>-23</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>E2*C2+(1-E2)*B2</f>
+        <v>48</v>
+      </c>
+      <c r="H2" s="62">
+        <f>AVERAGE(F3,F6:F7,F11)-AVERAGE(F2,F4:F5,F8:F10,F12:F13)</f>
+        <v>4.25</v>
+      </c>
+      <c r="I2" s="29">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J2" s="29">
+        <f>AVERAGE(B3,B6:B7,B11)</f>
+        <v>34</v>
+      </c>
+      <c r="K2" s="29">
+        <f>AVERAGE(B2,B4:B5,B8:B10,B12:B13)</f>
+        <v>39.5</v>
+      </c>
+      <c r="L2" s="29">
+        <f>AVERAGE(D2:D13)</f>
+        <v>-4.25</v>
+      </c>
+      <c r="M2" s="29">
+        <f>AVERAGE(D3,D6:D7,D11)</f>
+        <v>9.75</v>
+      </c>
+      <c r="N2" s="29">
+        <f>AVERAGE(D2,D4:D5,D8:D10,D12:D13)</f>
+        <v>-11.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2025,9 +2156,23 @@
       <c r="C3" s="6">
         <v>36</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
+        <v>36</v>
+      </c>
+      <c r="H3" s="65">
+        <f>L2+(J2-K2) + (1-I2)*(M2-N2)</f>
+        <v>4.2500000000000018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2037,9 +2182,19 @@
       <c r="C4" s="6">
         <v>33</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2049,9 +2204,22 @@
       <c r="C5" s="6">
         <v>31</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2061,9 +2229,22 @@
       <c r="C6" s="6">
         <v>55</v>
       </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2073,9 +2254,22 @@
       <c r="C7" s="6">
         <v>38</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2085,9 +2279,22 @@
       <c r="C8" s="6">
         <v>29</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>-7</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2097,9 +2304,19 @@
       <c r="C9" s="6">
         <v>23</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2109,9 +2326,22 @@
       <c r="C10" s="6">
         <v>34</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2121,9 +2351,22 @@
       <c r="C11" s="6">
         <v>46</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2133,9 +2376,22 @@
       <c r="C12" s="6">
         <v>27</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2145,44 +2401,71 @@
       <c r="C13" s="6">
         <v>24</v>
       </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>-23</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>109</v>
       </c>

</xml_diff>